<commit_message>
Removed default input form and created separate input file for each
</commit_message>
<xml_diff>
--- a/workitem_discovery_input_form.xlsx
+++ b/workitem_discovery_input_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsure\OneDrive\Documents\1_Official\DMAP\New_Development\DevOpsServer2020TOADO_Migration\multiple_project_repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3BE5D8-D9B8-4A33-9DED-454F0A3D3ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8409C7-A9C1-4D03-BB8D-96C64DF93420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Server URL</t>
   </si>
@@ -47,13 +47,7 @@
     <t>PAT</t>
   </si>
   <si>
-    <t>devserver</t>
-  </si>
-  <si>
     <t>http://172.191.4.85/TestCollection</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -334,7 +328,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -357,17 +351,14 @@
     </row>
     <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="2"/>
     </row>
   </sheetData>

</xml_diff>